<commit_message>
Frontend + Backend, Upload, Populate firebase, Fetching left to be done ...
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>14221a0566</t>
   </si>
@@ -46,12 +46,30 @@
   </si>
   <si>
     <t>regdNo</t>
+  </si>
+  <si>
+    <t>14221A0565</t>
+  </si>
+  <si>
+    <t>14221A0568</t>
+  </si>
+  <si>
+    <t>14221A0562</t>
+  </si>
+  <si>
+    <t>Aamir Shah</t>
+  </si>
+  <si>
+    <t>Shailendra</t>
+  </si>
+  <si>
+    <t>Pawan Aacharya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,10 +191,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="293338"/>
+        <a:sysClr val="windowText" lastClr="323F45"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="DADDDF"/>
+        <a:sysClr val="window" lastClr="E9EBEC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -431,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,102 +506,36 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>235</v>
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>1000</v>
+        <v>78990</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2345</v>
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>12000</v>
+        <v>89000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4657</v>
+      <c r="A7" t="s">
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>354</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>768</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>569</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2435</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9189389</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7328794</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>1200</v>
+        <v>9000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to make things work with heroku ... Hope this worjs
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>14221a0566</t>
   </si>
@@ -46,39 +46,6 @@
   </si>
   <si>
     <t>regdNo</t>
-  </si>
-  <si>
-    <t>14221A0565</t>
-  </si>
-  <si>
-    <t>14221A0568</t>
-  </si>
-  <si>
-    <t>14221A0562</t>
-  </si>
-  <si>
-    <t>Aamir Shah</t>
-  </si>
-  <si>
-    <t>Shailendra</t>
-  </si>
-  <si>
-    <t>Pawan Aacharya</t>
-  </si>
-  <si>
-    <t>14221A0502</t>
-  </si>
-  <si>
-    <t>14221A0512</t>
-  </si>
-  <si>
-    <t>14221A0563</t>
-  </si>
-  <si>
-    <t>Abhishek Putho</t>
-  </si>
-  <si>
-    <t>Some one with a name</t>
   </si>
 </sst>
 </file>
@@ -464,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C5" sqref="A5:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,66 +487,6 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>78990</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>89000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>